<commit_message>
added new country data for 2019 JEE
</commit_message>
<xml_diff>
--- a/data/JEE scores.xlsx
+++ b/data/JEE scores.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinemachalaba/Dropbox (EHA)/GHERI data sets to merge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahbaum/Dropbox (EHA)/GHERI AFRICOM/AFRICOM/4. Database/gheri-africom-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C173E47-3855-134E-B8D5-B68F159ABC58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256474A-A031-4444-ADD8-71EC2AA8CC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="460" windowWidth="27500" windowHeight="17540" xr2:uid="{71AF4992-C0C7-FE4A-A6A3-F0803508C14D}"/>
+    <workbookView xWindow="3960" yWindow="500" windowWidth="24120" windowHeight="15380" xr2:uid="{71AF4992-C0C7-FE4A-A6A3-F0803508C14D}"/>
   </bookViews>
   <sheets>
     <sheet name="JEE Scores" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="180">
   <si>
     <t>Country</t>
   </si>
@@ -520,15 +530,6 @@
   </si>
   <si>
     <t>Language - added</t>
-  </si>
-  <si>
-    <t>4 &amp; 1</t>
-  </si>
-  <si>
-    <t>3 &amp; 1</t>
-  </si>
-  <si>
-    <t>2 &amp; 1</t>
   </si>
   <si>
     <t>2016 - some with 2 assessments Country vs external experts</t>
@@ -651,7 +652,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,6 +753,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -765,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1063,6 +1070,24 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1380,9 +1405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5EBBD63-5F73-4C4D-BD76-6631FE42CC42}">
   <dimension ref="A1:BC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU73" sqref="AU73"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI33" sqref="AI33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1398,12 +1423,12 @@
     <col min="56" max="16384" width="11.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:55" s="21" customFormat="1" ht="181" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="70" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>0</v>
@@ -1442,13 +1467,13 @@
         <v>123</v>
       </c>
       <c r="O1" s="62" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P1" s="62" t="s">
         <v>124</v>
       </c>
       <c r="Q1" s="62" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="R1" s="62" t="s">
         <v>125</v>
@@ -1496,13 +1521,13 @@
         <v>139</v>
       </c>
       <c r="AG1" s="62" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AH1" s="62" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AI1" s="62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AJ1" s="62" t="s">
         <v>140</v>
@@ -1523,7 +1548,7 @@
         <v>145</v>
       </c>
       <c r="AP1" s="62" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AQ1" s="62" t="s">
         <v>146</v>
@@ -1535,7 +1560,7 @@
         <v>148</v>
       </c>
       <c r="AT1" s="62" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AU1" s="62" t="s">
         <v>149</v>
@@ -1570,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -1737,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>10</v>
@@ -1904,7 +1929,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>8</v>
@@ -2071,7 +2096,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>4</v>
@@ -2238,7 +2263,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>16</v>
@@ -2405,7 +2430,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>99</v>
@@ -2572,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>22</v>
@@ -2739,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>18</v>
@@ -2906,7 +2931,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>14</v>
@@ -3073,7 +3098,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>26</v>
@@ -3240,7 +3265,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>32</v>
@@ -3407,7 +3432,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>95</v>
@@ -3574,7 +3599,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>36</v>
@@ -3741,7 +3766,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>44</v>
@@ -3908,7 +3933,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>40</v>
@@ -4075,7 +4100,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>42</v>
@@ -4242,7 +4267,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>50</v>
@@ -4409,7 +4434,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>56</v>
@@ -4576,7 +4601,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>52</v>
@@ -4743,7 +4768,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>60</v>
@@ -4910,7 +4935,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>62</v>
@@ -5077,7 +5102,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>66</v>
@@ -5244,7 +5269,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>68</v>
@@ -5411,7 +5436,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>64</v>
@@ -5578,7 +5603,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>74</v>
@@ -5745,7 +5770,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>76</v>
@@ -5912,7 +5937,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>78</v>
@@ -6079,7 +6104,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>81</v>
@@ -6246,7 +6271,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>85</v>
@@ -6413,7 +6438,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>97</v>
@@ -6580,7 +6605,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>87</v>
@@ -6589,7 +6614,7 @@
         <v>88</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F32" s="13">
         <v>1</v>
@@ -6642,17 +6667,21 @@
       <c r="V32" s="46">
         <v>3</v>
       </c>
-      <c r="W32" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="X32" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y32" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z32" s="30" t="s">
-        <v>167</v>
+      <c r="W32" s="30">
+        <f>AVERAGE(4,1)</f>
+        <v>2.5</v>
+      </c>
+      <c r="X32" s="30">
+        <f>AVERAGE(3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="Y32" s="30">
+        <f>AVERAGE(3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="Z32" s="30">
+        <f>AVERAGE(2,1)</f>
+        <v>1.5</v>
       </c>
       <c r="AA32" s="40">
         <v>4</v>
@@ -6678,8 +6707,9 @@
       <c r="AH32" s="46">
         <v>3</v>
       </c>
-      <c r="AI32" s="30" t="s">
-        <v>167</v>
+      <c r="AI32" s="30">
+        <f>AVERAGE(2,1)</f>
+        <v>1.5</v>
       </c>
       <c r="AJ32" s="56">
         <v>1</v>
@@ -6747,7 +6777,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>109</v>
@@ -6914,7 +6944,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>91</v>
@@ -7081,7 +7111,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>101</v>
@@ -7248,7 +7278,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>107</v>
@@ -7415,7 +7445,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>111</v>
@@ -7582,7 +7612,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>113</v>
@@ -7749,7 +7779,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>54</v>
@@ -7916,7 +7946,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>58</v>
@@ -8083,7 +8113,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>89</v>
@@ -8250,7 +8280,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>105</v>
@@ -8403,7 +8433,7 @@
         <v>3</v>
       </c>
       <c r="BA42" s="52" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="BB42" s="16">
         <v>2</v>
@@ -8417,7 +8447,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>103</v>
@@ -8584,7 +8614,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>83</v>
@@ -8751,7 +8781,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>162</v>
@@ -8914,7 +8944,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C46" s="23" t="s">
         <v>24</v>
@@ -8938,7 +8968,9 @@
       <c r="L46" s="92"/>
       <c r="M46" s="92"/>
       <c r="N46" s="92"/>
-      <c r="O46" s="92"/>
+      <c r="O46" s="101">
+        <v>2</v>
+      </c>
       <c r="P46" s="90"/>
       <c r="Q46" s="20">
         <v>2</v>
@@ -9023,7 +9055,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>12</v>
@@ -9047,7 +9079,9 @@
       <c r="L47" s="93"/>
       <c r="M47" s="93"/>
       <c r="N47" s="93"/>
-      <c r="O47" s="93"/>
+      <c r="O47" s="102">
+        <v>1</v>
+      </c>
       <c r="P47" s="90"/>
       <c r="Q47" s="66">
         <v>1</v>
@@ -9132,7 +9166,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>20</v>
@@ -9156,7 +9190,9 @@
       <c r="L48" s="94"/>
       <c r="M48" s="94"/>
       <c r="N48" s="94"/>
-      <c r="O48" s="94"/>
+      <c r="O48" s="103">
+        <v>1</v>
+      </c>
       <c r="P48" s="90"/>
       <c r="Q48" s="87">
         <v>1</v>
@@ -9241,7 +9277,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C49" s="23" t="s">
         <v>38</v>
@@ -9265,7 +9301,9 @@
       <c r="L49" s="94"/>
       <c r="M49" s="94"/>
       <c r="N49" s="94"/>
-      <c r="O49" s="94"/>
+      <c r="O49" s="103">
+        <v>1</v>
+      </c>
       <c r="P49" s="90"/>
       <c r="Q49" s="87">
         <v>1</v>
@@ -9350,7 +9388,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>46</v>
@@ -9374,7 +9412,9 @@
       <c r="L50" s="95"/>
       <c r="M50" s="95"/>
       <c r="N50" s="95"/>
-      <c r="O50" s="96"/>
+      <c r="O50" s="104">
+        <v>2</v>
+      </c>
       <c r="P50" s="90"/>
       <c r="Q50" s="55">
         <v>1</v>
@@ -9459,7 +9499,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>70</v>
@@ -9483,7 +9523,9 @@
       <c r="L51" s="93"/>
       <c r="M51" s="93"/>
       <c r="N51" s="92"/>
-      <c r="O51" s="92"/>
+      <c r="O51" s="101">
+        <v>1</v>
+      </c>
       <c r="P51" s="90"/>
       <c r="Q51" s="19">
         <v>1</v>
@@ -9568,7 +9610,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="73" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>93</v>
@@ -9592,7 +9634,9 @@
       <c r="L52" s="97"/>
       <c r="M52" s="97"/>
       <c r="N52" s="97"/>
-      <c r="O52" s="97"/>
+      <c r="O52" s="105">
+        <v>1</v>
+      </c>
       <c r="P52" s="90"/>
       <c r="Q52" s="56">
         <v>1</v>
@@ -9677,7 +9721,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="73" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>2</v>
@@ -9685,158 +9729,158 @@
       <c r="D53" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>169</v>
+      <c r="E53" s="13">
+        <v>2019</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O53" s="100">
+        <v>2</v>
       </c>
       <c r="P53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q53" s="100">
+        <v>2</v>
       </c>
       <c r="R53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S53" s="100">
+        <v>1</v>
+      </c>
+      <c r="T53" s="100">
+        <v>1</v>
       </c>
       <c r="U53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V53" s="100">
+        <v>3</v>
+      </c>
+      <c r="W53" s="100">
+        <v>2</v>
+      </c>
+      <c r="X53" s="100">
+        <v>2</v>
       </c>
       <c r="Y53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z53" s="100">
+        <v>2</v>
       </c>
       <c r="AA53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE53" s="100">
+        <v>2</v>
+      </c>
+      <c r="AF53" s="100">
+        <v>2</v>
       </c>
       <c r="AG53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH53" s="100">
+        <v>2</v>
+      </c>
+      <c r="AI53" s="100">
+        <v>2</v>
       </c>
       <c r="AJ53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP53" s="100">
+        <v>3</v>
       </c>
       <c r="AQ53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT53" s="100">
+        <v>3</v>
       </c>
       <c r="AU53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX53" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX53" s="100">
+        <v>2</v>
+      </c>
+      <c r="AY53" s="100">
+        <v>1</v>
       </c>
       <c r="AZ53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC53" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9844,7 +9888,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>28</v>
@@ -9853,157 +9897,157 @@
         <v>29</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX54" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX54" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY54" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC54" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -10011,7 +10055,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>30</v>
@@ -10020,157 +10064,157 @@
         <v>31</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX55" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY55" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC55" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -10178,7 +10222,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>34</v>
@@ -10187,157 +10231,157 @@
         <v>35</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX56" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX56" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY56" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC56" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -10345,7 +10389,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>48</v>
@@ -10354,157 +10398,157 @@
         <v>49</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX57" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX57" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY57" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC57" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:55" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10512,7 +10556,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>72</v>
@@ -10521,157 +10565,157 @@
         <v>73</v>
       </c>
       <c r="E58" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX58" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX58" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY58" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC58" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:55" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10679,166 +10723,166 @@
         <v>58</v>
       </c>
       <c r="B59" s="73" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>80</v>
       </c>
       <c r="E59" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="O59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="O59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="P59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Q59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="R59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="S59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="T59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="S59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="T59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="U59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="V59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="W59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="X59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="V59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="W59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="X59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="Y59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="Z59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AA59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AB59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AE59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AE59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AG59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AH59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AH59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AJ59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AK59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AL59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AM59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AN59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AO59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AP59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AP59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AQ59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AR59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AS59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AT59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AT59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AU59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AV59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AW59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AX59" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AY59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="AX59" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AY59" s="100" t="s">
+        <v>166</v>
       </c>
       <c r="AZ59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BA59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BB59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="BC59" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>